<commit_message>
Match inventory.xlsx to tests/shares
</commit_message>
<xml_diff>
--- a/tests/inventories/Digital Production Hub Inventory.xlsx
+++ b/tests/inventories/Digital Production Hub Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\hub-audit\tests\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5677043-653E-4953-BA59-1373D55D2793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40AE624-48C5-453F-AEDB-6D0852DD4777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="105" windowWidth="27975" windowHeight="20235" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24705" yWindow="645" windowWidth="26895" windowHeight="20235" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'C'!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Extra!$A$1:$G$169</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">mezz_one!$A$1:$F$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Second_Level!$A$1:$F$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Second_Level!$A$1:$F$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Top!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
   <si>
     <t>Share (required)</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Working Files</t>
   </si>
   <si>
-    <t>Prepping files for indexing</t>
-  </si>
-  <si>
     <t>Backlog</t>
   </si>
   <si>
@@ -110,18 +107,12 @@
     <t>permanent</t>
   </si>
   <si>
-    <t>3 months after download date (in folder title)</t>
-  </si>
-  <si>
     <t>Permanent</t>
   </si>
   <si>
     <t>Transfer</t>
   </si>
   <si>
-    <t>Medium Priority</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -155,18 +143,9 @@
     <t>Camila</t>
   </si>
   <si>
-    <t>6 months</t>
-  </si>
-  <si>
-    <t>1 year</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>E_1</t>
   </si>
   <si>
@@ -188,24 +167,9 @@
     <t>S_1</t>
   </si>
   <si>
-    <t>S_2</t>
-  </si>
-  <si>
-    <t>S_3</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Sam</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>T_1</t>
   </si>
   <si>
@@ -222,6 +186,33 @@
   </si>
   <si>
     <t>1 week</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Second_Level</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>S_2\S_2a</t>
+  </si>
+  <si>
+    <t>S_2\S_2b</t>
+  </si>
+  <si>
+    <t>S_3\S_3a</t>
+  </si>
+  <si>
+    <t>S_3\S_3b</t>
   </si>
 </sst>
 </file>
@@ -299,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,9 +302,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,9 +624,9 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,22 +687,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3">
-        <v>45474</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+        <v>45292</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -744,7 +730,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,19 +791,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -838,11 +818,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,56 +883,90 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
+      <c r="E3" s="3">
+        <v>81893</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
+      <c r="E4" s="3">
+        <v>81893</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" s="3">
+        <v>81893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3">
+        <v>81893</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +991,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,36 +1052,36 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>82212</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3">
-        <v>45688</v>
+        <v>82212</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1679,7 +1693,7 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" customWidth="1"/>
     <col min="6" max="6" width="107.5703125" bestFit="1" customWidth="1"/>
@@ -1689,7 +1703,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1709,7 +1723,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1727,23 +1741,23 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
+      <c r="B4" s="9"/>
       <c r="E4" s="3"/>
     </row>
   </sheetData>
@@ -1765,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF5D498-3B84-4311-8ABA-A02E638C435F}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,16 +1840,16 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="E3" s="3">
+        <v>82272</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1843,16 +1857,16 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="E4" s="3">
+        <v>82272</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,23 +1874,51 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="E5" s="3">
+        <v>82272</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="3"/>
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3">
+        <v>82272</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3">
+        <v>82272</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
@@ -1923,10 +1965,13 @@
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
     </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F22" xr:uid="{BAF5D498-3B84-4311-8ABA-A02E638C435F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F21">
-    <sortCondition ref="B3:B21"/>
+  <autoFilter ref="A1:F23" xr:uid="{BAF5D498-3B84-4311-8ABA-A02E638C435F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F22">
+    <sortCondition ref="B3:B22"/>
   </sortState>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{70EA0589-FE86-428B-A9B8-845CEE32FFE0}">
@@ -1942,11 +1987,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,36 +2052,36 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2057,6 +2102,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
+      <UserInfo>
+        <DisplayName>Mary K Willoughby</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Steven G Armour</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Adriane M Hanson</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kathryn Manis</DisplayName>
+        <AccountId>190</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051E6EA1095A24B4CB9729835D0C20D83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc0c55b87092411a2e066e82a5a276b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d09f93eb-00d0-400e-a5cd-81161df8bdb0" xmlns:ns3="603b486a-d1d5-4102-bae7-ac15bf6ef37a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5e422eacb72394920a94c0663222dde" ns2:_="" ns3:_="">
     <xsd:import namespace="d09f93eb-00d0-400e-a5cd-81161df8bdb0"/>
@@ -2279,45 +2362,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
-      <UserInfo>
-        <DisplayName>Mary K Willoughby</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Steven G Armour</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Adriane M Hanson</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kathryn Manis</DisplayName>
-        <AccountId>190</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77D5365D-8015-4AE9-A41D-CA09BCDCE43E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2334,22 +2397,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Split Audit_Result to 3 columns
Having a different column for each audit type for easier review and easier dataframe updates. Also simplified the text used for errors.
</commit_message>
<xml_diff>
--- a/tests/inventories/Digital Production Hub Inventory.xlsx
+++ b/tests/inventories/Digital Production Hub Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\hub-audit\tests\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40AE624-48C5-453F-AEDB-6D0852DD4777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42739EA3-0B9E-49E4-ADE1-8ECC4C7E5969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24705" yWindow="645" windowWidth="26895" windowHeight="20235" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20610" yWindow="975" windowWidth="26895" windowHeight="20235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="54">
   <si>
     <t>Share (required)</t>
   </si>
@@ -728,9 +728,9 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,9 +795,6 @@
       </c>
       <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF5D498-3B84-4311-8ABA-A02E638C435F}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2102,44 +2099,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
-      <UserInfo>
-        <DisplayName>Mary K Willoughby</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Steven G Armour</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Adriane M Hanson</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kathryn Manis</DisplayName>
-        <AccountId>190</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051E6EA1095A24B4CB9729835D0C20D83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc0c55b87092411a2e066e82a5a276b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d09f93eb-00d0-400e-a5cd-81161df8bdb0" xmlns:ns3="603b486a-d1d5-4102-bae7-ac15bf6ef37a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5e422eacb72394920a94c0663222dde" ns2:_="" ns3:_="">
     <xsd:import namespace="d09f93eb-00d0-400e-a5cd-81161df8bdb0"/>
@@ -2362,25 +2321,45 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
+      <UserInfo>
+        <DisplayName>Mary K Willoughby</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Steven G Armour</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Adriane M Hanson</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kathryn Manis</DisplayName>
+        <AccountId>190</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77D5365D-8015-4AE9-A41D-CA09BCDCE43E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2397,4 +2376,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sync test_script with new test data
</commit_message>
<xml_diff>
--- a/tests/inventories/Digital Production Hub Inventory.xlsx
+++ b/tests/inventories/Digital Production Hub Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\hub-audit\tests\inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahanson\Documents\GitHub\hub-audit\tests\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42739EA3-0B9E-49E4-ADE1-8ECC4C7E5969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E50EA96-B4BF-4A88-919D-01E2848C2723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="975" windowWidth="26895" windowHeight="20235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
@@ -42,8 +42,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="56">
   <si>
     <t>Share (required)</t>
   </si>
@@ -213,6 +211,12 @@
   </si>
   <si>
     <t>S_3\S_3b</t>
+  </si>
+  <si>
+    <t>T_Hub</t>
+  </si>
+  <si>
+    <t>Include.txt</t>
   </si>
 </sst>
 </file>
@@ -323,9 +327,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -363,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -469,7 +473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -611,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -629,17 +633,17 @@
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="118" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -685,7 +689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -702,10 +706,10 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E5" s="3"/>
     </row>
   </sheetData>
@@ -728,22 +732,22 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="118" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -789,7 +793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -822,17 +826,17 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="118" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -878,7 +882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -895,7 +899,7 @@
         <v>81893</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -912,7 +916,7 @@
         <v>81893</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -929,7 +933,7 @@
         <v>81893</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -946,7 +950,7 @@
         <v>81893</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -991,17 +995,17 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="118" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>82212</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1081,585 +1085,585 @@
         <v>82212</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B19" s="4"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B20" s="4"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B21" s="4"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.75">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B27" s="5"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B28" s="5"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B29" s="5"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B30" s="5"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B31" s="5"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B32" s="5"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B33" s="5"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B34" s="5"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B35" s="5"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B36" s="5"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B37" s="5"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B38" s="5"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B39" s="5"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B40" s="5"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B41" s="5"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B42" s="5"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B43" s="5"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B44" s="5"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B56" s="5"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B57" s="5"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B58" s="5"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B59" s="5"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B60" s="5"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B61" s="5"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B62" s="5"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B63" s="5"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B64" s="5"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B67" s="5"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B68" s="5"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B69" s="5"/>
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B70" s="5"/>
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B71" s="5"/>
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B72" s="5"/>
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B73" s="5"/>
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B74" s="5"/>
       <c r="E74" s="3"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B75" s="5"/>
       <c r="E75" s="3"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B76" s="5"/>
       <c r="E76" s="3"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B77" s="5"/>
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B78" s="5"/>
       <c r="E78" s="3"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E80" s="3"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E81" s="3"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B82" s="5"/>
       <c r="E82" s="3"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B83" s="5"/>
       <c r="E83" s="3"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B84" s="5"/>
       <c r="E84" s="3"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B85" s="5"/>
       <c r="E85" s="3"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B86" s="5"/>
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B87" s="5"/>
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B88" s="5"/>
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B89" s="5"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B90" s="5"/>
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B91" s="5"/>
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B92" s="5"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B93" s="5"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B94" s="5"/>
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B95" s="5"/>
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B96" s="5"/>
       <c r="E96" s="3"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B97" s="5"/>
       <c r="E97" s="3"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B98" s="5"/>
       <c r="E98" s="3"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B99" s="5"/>
       <c r="E99" s="3"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B100" s="5"/>
       <c r="E100" s="3"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B101" s="5"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B102" s="5"/>
       <c r="E102" s="3"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E103" s="3"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.75">
       <c r="E106" s="8"/>
     </row>
-    <row r="107" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.75">
       <c r="E107" s="8"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E108" s="3"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.75">
       <c r="E109" s="3"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B111" s="5"/>
       <c r="E111" s="3"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B112" s="5"/>
       <c r="E112" s="3"/>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B113" s="5"/>
       <c r="E113" s="3"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B114" s="5"/>
       <c r="E114" s="3"/>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B115" s="5"/>
       <c r="E115" s="3"/>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B116" s="5"/>
       <c r="E116" s="3"/>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B117" s="5"/>
       <c r="E117" s="3"/>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B118" s="5"/>
       <c r="E118" s="3"/>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B119" s="5"/>
       <c r="E119" s="3"/>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B120" s="5"/>
       <c r="E120" s="3"/>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B121" s="5"/>
       <c r="E121" s="3"/>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B122" s="5"/>
       <c r="E122" s="3"/>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B123" s="5"/>
       <c r="E123" s="3"/>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B124" s="5"/>
       <c r="E124" s="3"/>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B125" s="5"/>
       <c r="E125" s="3"/>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B126" s="5"/>
       <c r="E126" s="3"/>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B127" s="5"/>
       <c r="E127" s="3"/>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.75">
       <c r="B128" s="5"/>
       <c r="E128" s="3"/>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B129" s="5"/>
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B130" s="5"/>
       <c r="E130" s="3"/>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B131" s="5"/>
       <c r="E131" s="3"/>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B132" s="5"/>
       <c r="E132" s="3"/>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B133" s="5"/>
       <c r="E133" s="3"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B134" s="5"/>
       <c r="E134" s="3"/>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B135" s="5"/>
       <c r="E135" s="3"/>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B136" s="5"/>
       <c r="E136" s="3"/>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B137" s="5"/>
       <c r="E137" s="3"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B138" s="5"/>
       <c r="E138" s="3"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B139" s="5"/>
       <c r="E139" s="3"/>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B140" s="5"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.75">
       <c r="E141" s="3"/>
       <c r="G141" s="3"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B142" s="5"/>
       <c r="E142" s="3"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.75">
       <c r="E143" s="3"/>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.75">
       <c r="E144" s="3"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E145" s="3"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E146" s="3"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E147" s="3"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E148" s="3"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E149" s="3"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E150" s="3"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E151" s="3"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E152" s="3"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E153" s="3"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E154" s="3"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E155" s="3"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E156" s="3"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E158" s="3"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E159" s="3"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E160" s="3"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E161" s="3"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E162" s="3"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E163" s="3"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E164" s="3"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E165" s="3"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E166" s="3"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E167" s="3"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E168" s="3"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E169" s="3"/>
     </row>
   </sheetData>
@@ -1687,16 +1691,16 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="107.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="107.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1736,7 +1740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1753,7 +1757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="B4" s="9"/>
       <c r="E4" s="3"/>
     </row>
@@ -1782,17 +1786,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="2" width="33.40625" customWidth="1"/>
+    <col min="3" max="3" width="35.1328125" customWidth="1"/>
+    <col min="4" max="4" width="41.40625" customWidth="1"/>
+    <col min="5" max="5" width="29.86328125" customWidth="1"/>
+    <col min="6" max="6" width="25.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1849,7 +1853,7 @@
         <v>82272</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1866,7 +1870,7 @@
         <v>82272</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>82272</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>82272</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1917,52 +1921,52 @@
         <v>82272</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.75">
       <c r="E23" s="3"/>
     </row>
   </sheetData>
@@ -1984,24 +1988,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="78.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="43.40625" customWidth="1"/>
+    <col min="6" max="6" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="118" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +2051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -2078,6 +2082,40 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2099,6 +2137,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
+      <UserInfo>
+        <DisplayName>Mary K Willoughby</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Steven G Armour</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Adriane M Hanson</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kathryn Manis</DisplayName>
+        <AccountId>190</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051E6EA1095A24B4CB9729835D0C20D83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc0c55b87092411a2e066e82a5a276b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d09f93eb-00d0-400e-a5cd-81161df8bdb0" xmlns:ns3="603b486a-d1d5-4102-bae7-ac15bf6ef37a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5e422eacb72394920a94c0663222dde" ns2:_="" ns3:_="">
     <xsd:import namespace="d09f93eb-00d0-400e-a5cd-81161df8bdb0"/>
@@ -2321,45 +2397,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
-      <UserInfo>
-        <DisplayName>Mary K Willoughby</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Steven G Armour</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Adriane M Hanson</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kathryn Manis</DisplayName>
-        <AccountId>190</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77D5365D-8015-4AE9-A41D-CA09BCDCE43E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2376,22 +2432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Examples sheet to test files
</commit_message>
<xml_diff>
--- a/tests/inventories/Digital Production Hub Inventory.xlsx
+++ b/tests/inventories/Digital Production Hub Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahanson\Documents\GitHub\hub-audit\tests\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E50EA96-B4BF-4A88-919D-01E2848C2723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FD102D-33EF-4F05-BF5D-85142F120449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="mezz_one" sheetId="6" r:id="rId5"/>
     <sheet name="Second_Level" sheetId="14" r:id="rId6"/>
     <sheet name="Top" sheetId="8" r:id="rId7"/>
+    <sheet name="Examples" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A!$A$1:$G$2</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="59">
   <si>
     <t>Share (required)</t>
   </si>
@@ -217,6 +218,15 @@
   </si>
   <si>
     <t>Include.txt</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>E. X. Ample</t>
+  </si>
+  <si>
+    <t>Info</t>
   </si>
 </sst>
 </file>
@@ -1990,9 +2000,9 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2136,45 +2146,113 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
-      <UserInfo>
-        <DisplayName>Mary K Willoughby</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Steven G Armour</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Adriane M Hanson</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kathryn Manis</DisplayName>
-        <AccountId>190</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32071C51-F277-4A5C-95F8-B0AD81BA1624}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="7" width="21.31640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="191.75" x14ac:dyDescent="0.75">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45688</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45688</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0CD18758-2B70-40F5-BA68-94C66ACE1EBF}">
+      <formula1>"Access/Mezzanine,Backlog,Outsourced Graphics,Medium Priority,Transfer,Working Files"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051E6EA1095A24B4CB9729835D0C20D83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc0c55b87092411a2e066e82a5a276b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d09f93eb-00d0-400e-a5cd-81161df8bdb0" xmlns:ns3="603b486a-d1d5-4102-bae7-ac15bf6ef37a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5e422eacb72394920a94c0663222dde" ns2:_="" ns3:_="">
     <xsd:import namespace="d09f93eb-00d0-400e-a5cd-81161df8bdb0"/>
@@ -2397,25 +2475,45 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="603b486a-d1d5-4102-bae7-ac15bf6ef37a">
+      <UserInfo>
+        <DisplayName>Mary K Willoughby</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Steven G Armour</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Adriane M Hanson</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kathryn Manis</DisplayName>
+        <AccountId>190</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77D5365D-8015-4AE9-A41D-CA09BCDCE43E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2432,4 +2530,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{014E67E0-5B31-4AB8-94C2-FDAC36674AC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31CFD876-DDBA-4209-BCCE-053DBDF40974}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="603b486a-d1d5-4102-bae7-ac15bf6ef37a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>